<commit_message>
all data inserted into cells
</commit_message>
<xml_diff>
--- a/categorized.xlsx
+++ b/categorized.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="DQAC"/>
@@ -16,23 +16,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>2022-2023</t>
   </si>
+  <si>
+    <t>Conference Presentation</t>
+  </si>
+  <si>
+    <t>Journal Publication-Non Indexed</t>
+  </si>
+  <si>
+    <t>fdp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,7 +58,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -55,12 +77,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -365,42 +396,67 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
control width of cells
</commit_message>
<xml_diff>
--- a/categorized.xlsx
+++ b/categorized.xlsx
@@ -423,7 +423,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,7 +464,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
fixed alignment of year column
</commit_message>
<xml_diff>
--- a/categorized.xlsx
+++ b/categorized.xlsx
@@ -48,8 +48,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,7 +431,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>2022-2023</t>
         </is>
@@ -469,7 +472,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>2022-2023</t>
         </is>

</xml_diff>

<commit_message>
some test cases in excel
</commit_message>
<xml_diff>
--- a/categorized.xlsx
+++ b/categorized.xlsx
@@ -1,36 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Samuel\6CME\Project_DriveReader\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62145D7E-7EBA-4150-ACC9-1351E51D7F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DQAC" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="RESEARCH" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="exempted" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="DQAC" sheetId="1" r:id="rId1"/>
+    <sheet name="RESEARCH" sheetId="2" r:id="rId2"/>
+    <sheet name="exempted" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>fdp</t>
+  </si>
+  <si>
+    <t>Conference Presentation</t>
+  </si>
+  <si>
+    <t>Journal Publication-Non Indexed</t>
+  </si>
+  <si>
+    <t>READ_ME.xlsx</t>
+  </si>
+  <si>
+    <t>CUCS - Research</t>
+  </si>
+  <si>
+    <t>Readme.txt</t>
+  </si>
+  <si>
+    <t>20220915_achs_rv_1.pdf</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -48,84 +81,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,35 +388,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
+    <col min="1" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>2022-2023</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>fdp</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
     </row>
@@ -454,45 +420,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="31" customWidth="1" min="2" max="2"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>2022-2023</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Conference Presentation</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Journal Publication-Non Indexed</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
@@ -505,53 +462,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>READ_ME.xlsx</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CUCS - Research</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Readme.txt</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CUCS - Research</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>20220915_achs_rv_1.pdf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CUCS - Research</t>
-        </is>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are now arranged alphabetically in categorized
</commit_message>
<xml_diff>
--- a/categorized.xlsx
+++ b/categorized.xlsx
@@ -522,11 +522,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mou s</t>
+          <t>Book Chapter</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -536,13 +536,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Book Chapter</t>
+          <t>Journal Publication-Indexed</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -552,11 +552,11 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Journal Publication-Indexed</t>
+          <t>Mou s</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -592,7 +592,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mou s</t>
+          <t>Book Chapter</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -602,11 +602,11 @@
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Conference Session Chair</t>
+          <t>Conference Attended</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -622,11 +622,11 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conference Attended</t>
+          <t>Conference Presentation</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -642,7 +642,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Book Chapter</t>
+          <t>Conference Session Chair</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -652,17 +652,17 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Patent Filed</t>
+          <t>Journal Publication-Indexed</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Journal Publication-Indexed</t>
+          <t>Journal Publication-Non Indexed</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -672,7 +672,7 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>Seminar Organized</t>
+          <t>Mou s</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -682,7 +682,7 @@
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>Journal Publication-Non Indexed</t>
+          <t>Patent Filed</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -692,11 +692,11 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>Conference Presentation</t>
+          <t>Seminar Organized</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>